<commit_message>
I approve this message
</commit_message>
<xml_diff>
--- a/data/dragonfly.xlsx
+++ b/data/dragonfly.xlsx
@@ -106,7 +106,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -115,6 +116,7 @@
           <c:tx>
             <c:v>DF1</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$1:$C$100</c:f>
@@ -431,6 +433,7 @@
           <c:tx>
             <c:v>DF2</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$101:$C$200</c:f>
@@ -747,6 +750,7 @@
           <c:tx>
             <c:v>DF3</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$201:$C$300</c:f>
@@ -1063,6 +1067,7 @@
           <c:tx>
             <c:v>DF4</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$301:$C$400</c:f>
@@ -1379,6 +1384,7 @@
           <c:tx>
             <c:v>DF5</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$401:$C$500</c:f>
@@ -1695,6 +1701,7 @@
           <c:tx>
             <c:v>DF6</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$501:$C$600</c:f>
@@ -2011,6 +2018,7 @@
           <c:tx>
             <c:v>DF7</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>dragonfly.csv!$C$601:$C$700</c:f>
@@ -2327,6 +2335,7 @@
           <c:tx>
             <c:v>DF8</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -2345,9 +2354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
         <c:axId val="2136611176"/>
         <c:axId val="2136259480"/>
-      </c:areaChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="2136611176"/>
         <c:scaling>
@@ -2379,7 +2390,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2136611176"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2409,10 +2420,10 @@
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>74930</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>